<commit_message>
Unidade de controle finalizada
</commit_message>
<xml_diff>
--- a/Part 2 - Processor Project/Controladora.xlsx
+++ b/Part 2 - Processor Project/Controladora.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a5b9f3a93ad922a/Documentos/UFMG/7-PERIODO/LABORATÓRIO DE ARQUITETURA E ORGANIZAÇÃO DE COMPUTADORES/Projeto de Processador/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a5b9f3a93ad922a/Documentos/UFMG/7-PERIODO/LABORATÓRIO DE ARQUITETURA E ORGANIZAÇÃO DE COMPUTADORES/Lab_AOC/Part 2 - Processor Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="241" documentId="11_AD4D361C20488DEA4E38A0D48C9A590A5BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3576F59-0CA2-4BC6-866C-D8A63D4B4E89}"/>
+  <xr:revisionPtr revIDLastSave="253" documentId="11_AD4D361C20488DEA4E38A0D48C9A590A5BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82946EBA-4B37-4338-B24B-E8945D7579CB}"/>
   <bookViews>
-    <workbookView xWindow="-16200" yWindow="-12060" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16305" yWindow="1500" windowWidth="16410" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -546,7 +546,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,11 +556,10 @@
     <col min="3" max="3" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="9.140625" style="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.140625" style="1"/>
     <col min="14" max="14" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -582,16 +581,16 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>3</v>
@@ -615,16 +614,16 @@
         <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>51</v>
@@ -650,16 +649,16 @@
         <v>33</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>9</v>
@@ -685,16 +684,16 @@
         <v>32</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>10</v>
@@ -720,16 +719,16 @@
         <v>32</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>11</v>
@@ -755,16 +754,16 @@
         <v>32</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>12</v>
@@ -790,16 +789,16 @@
         <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>13</v>
@@ -825,16 +824,16 @@
         <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>14</v>
@@ -860,16 +859,16 @@
         <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>15</v>
@@ -895,16 +894,16 @@
         <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>16</v>
@@ -930,16 +929,16 @@
         <v>33</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>17</v>
@@ -965,16 +964,16 @@
         <v>33</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>18</v>
@@ -1000,16 +999,16 @@
         <v>33</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>19</v>
@@ -1035,16 +1034,16 @@
         <v>32</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>20</v>
@@ -1070,16 +1069,16 @@
         <v>33</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>21</v>
@@ -1105,16 +1104,16 @@
         <v>33</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>22</v>
@@ -1140,16 +1139,16 @@
         <v>33</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>23</v>
@@ -1175,16 +1174,16 @@
         <v>52</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>24</v>
@@ -1210,16 +1209,16 @@
         <v>52</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1239,16 +1238,16 @@
         <v>32</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1268,16 +1267,16 @@
         <v>32</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1297,16 +1296,16 @@
         <v>32</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1326,16 +1325,16 @@
         <v>52</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1355,16 +1354,16 @@
         <v>52</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1373,6 +1372,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="E8" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Somador Branch e Teste do Código Binário
</commit_message>
<xml_diff>
--- a/Part 2 - Processor Project/Controladora.xlsx
+++ b/Part 2 - Processor Project/Controladora.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a5b9f3a93ad922a/Documentos/UFMG/7-PERIODO/LABORATÓRIO DE ARQUITETURA E ORGANIZAÇÃO DE COMPUTADORES/Lab_AOC/Part 2 - Processor Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="253" documentId="11_AD4D361C20488DEA4E38A0D48C9A590A5BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82946EBA-4B37-4338-B24B-E8945D7579CB}"/>
+  <xr:revisionPtr revIDLastSave="257" documentId="11_AD4D361C20488DEA4E38A0D48C9A590A5BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{444A0509-1D61-46CA-862F-8C3C4906B5C0}"/>
   <bookViews>
-    <workbookView xWindow="-16305" yWindow="1500" windowWidth="16410" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="75" yWindow="4245" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -546,7 +546,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>